<commit_message>
added support for mutliple xlsx files
</commit_message>
<xml_diff>
--- a/Wedstrijden.xlsx
+++ b/Wedstrijden.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14310" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="11670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kogelslinger wedstrijden" sheetId="1" r:id="rId1"/>
     <sheet name="Competitie 2020" sheetId="2" r:id="rId2"/>
+    <sheet name="gewichten" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="32">
   <si>
     <t>Kogelslinger wedstrijden</t>
   </si>
@@ -63,6 +64,54 @@
   </si>
   <si>
     <t>Sen</t>
+  </si>
+  <si>
+    <t>kogelslingeren</t>
+  </si>
+  <si>
+    <t>categorie</t>
+  </si>
+  <si>
+    <t>gewicht</t>
+  </si>
+  <si>
+    <t>JD</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>JB</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>JA</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>HEREN</t>
+  </si>
+  <si>
+    <t>DAMES</t>
+  </si>
+  <si>
+    <t>gewichtwerpen</t>
+  </si>
+  <si>
+    <t>discuswerpen</t>
+  </si>
+  <si>
+    <t>kogelsltoten</t>
   </si>
 </sst>
 </file>
@@ -70,13 +119,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_(&quot;€&quot;\ * #,##0.00_);_(&quot;€&quot;\ * \(#,##0.00\);_(&quot;€&quot;\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;€&quot;\ * #,##0_);_(&quot;€&quot;\ * \(#,##0\);_(&quot;€&quot;\ * &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_(&quot;€&quot;\ * #,##0.00_);_(&quot;€&quot;\ * \(#,##0.00\);_(&quot;€&quot;\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(&quot;€&quot;\ * #,##0_);_(&quot;€&quot;\ * \(#,##0\);_(&quot;€&quot;\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -88,33 +143,28 @@
       <charset val="0"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <charset val="0"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -136,7 +186,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,6 +223,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -166,9 +270,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,74 +298,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -259,31 +308,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,151 +488,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,6 +499,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -462,11 +526,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -486,17 +556,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -512,17 +571,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -536,24 +589,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -561,137 +610,144 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1034,23 +1090,23 @@
   </cols>
   <sheetData>
     <row r="1" ht="20.25" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="6">
         <v>43869</v>
       </c>
       <c r="B3" t="s">
@@ -1061,7 +1117,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="6">
         <v>43932</v>
       </c>
       <c r="B4" t="s">
@@ -1072,48 +1128,48 @@
       </c>
     </row>
     <row r="28" ht="20.25" spans="1:1">
-      <c r="A28" s="1"/>
+      <c r="A28" s="4"/>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="3"/>
+      <c r="A30" s="6"/>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="3"/>
-      <c r="C31" s="4"/>
+      <c r="A31" s="6"/>
+      <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="3"/>
-      <c r="C32" s="4"/>
+      <c r="A32" s="6"/>
+      <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="3"/>
+      <c r="A33" s="6"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="3"/>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="3"/>
-      <c r="C35" s="4"/>
+      <c r="A35" s="6"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="3"/>
+      <c r="A36" s="6"/>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="3"/>
+      <c r="A37" s="6"/>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="3"/>
+      <c r="A38" s="6"/>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="3"/>
+      <c r="A39" s="6"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="3"/>
+      <c r="A40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1127,7 +1183,7 @@
   <sheetPr/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1139,23 +1195,23 @@
   </cols>
   <sheetData>
     <row r="1" ht="20.25" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3">
+      <c r="A3" s="6">
         <v>43939</v>
       </c>
       <c r="C3" t="s">
@@ -1163,31 +1219,31 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3">
+      <c r="A4" s="6">
         <v>43960</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3">
+      <c r="A5" s="6">
         <v>43995</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="3">
+      <c r="A7" s="6">
         <v>43940</v>
       </c>
       <c r="C7" t="s">
@@ -1195,7 +1251,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="3">
+      <c r="A8" s="6">
         <v>43954</v>
       </c>
       <c r="C8" t="s">
@@ -1203,23 +1259,23 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>43989</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="3">
+      <c r="A11" s="6">
         <v>43968</v>
       </c>
       <c r="C11" t="s">
@@ -1227,7 +1283,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="3">
+      <c r="A12" s="6">
         <v>44003</v>
       </c>
       <c r="C12" t="s">
@@ -1235,7 +1291,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
@@ -1243,7 +1299,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="3">
+      <c r="A14" s="6">
         <v>43947</v>
       </c>
       <c r="C14" t="s">
@@ -1251,7 +1307,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="3">
+      <c r="A15" s="6">
         <v>43975</v>
       </c>
       <c r="C15" t="s">
@@ -1259,7 +1315,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="3">
+      <c r="A16" s="6">
         <v>44017</v>
       </c>
       <c r="C16" t="s">
@@ -1271,4 +1327,378 @@
   <pageSetup paperSize="1" orientation="portrait" horizontalDpi="600"/>
   <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="3" max="3" width="3.57142857142857" customWidth="1"/>
+    <col min="4" max="4" width="9.71428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7.26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <v>7.26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9.08</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3">
+        <v>5.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="D14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="3">
+        <v>7.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3">
+        <v>15.88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="3">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="3">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="3">
+        <v>7.26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>